<commit_message>
merging and checking data
</commit_message>
<xml_diff>
--- a/data/davis matches/davis_2014.xlsx
+++ b/data/davis matches/davis_2014.xlsx
@@ -749,7 +749,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>58</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr"/>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>58</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -1120,7 +1120,7 @@
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>40</t>
         </is>
       </c>
       <c r="AB7" t="n">
@@ -1284,12 +1284,12 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>718</t>
+          <t>716</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>912</t>
+          <t>1010</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr"/>
@@ -1372,12 +1372,12 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>1163</t>
+          <t>1194</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>1371=</t>
+          <t>1364=</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr"/>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>222</t>
         </is>
       </c>
       <c r="X12" t="inlineStr"/>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>222</t>
         </is>
       </c>
       <c r="X16" t="inlineStr"/>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>286</t>
         </is>
       </c>
       <c r="AB16" t="n">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>222</t>
         </is>
       </c>
       <c r="X18" t="inlineStr"/>
@@ -2861,7 +2861,7 @@
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr">
         <is>
-          <t>1765</t>
+          <t>1774</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>136</t>
         </is>
       </c>
       <c r="X30" t="inlineStr"/>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="W34" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>136</t>
         </is>
       </c>
       <c r="X34" t="inlineStr"/>
@@ -3696,12 +3696,12 @@
       </c>
       <c r="W37" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>86</t>
         </is>
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>228</t>
+          <t>224</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr"/>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="W40" t="inlineStr">
         <is>
-          <t>1337=</t>
+          <t>1350=</t>
         </is>
       </c>
       <c r="X40" t="inlineStr"/>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr"/>
@@ -5096,7 +5096,7 @@
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="AB53" t="n">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="X55" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr"/>
@@ -5533,7 +5533,7 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>164</t>
         </is>
       </c>
       <c r="Y58" t="inlineStr"/>
@@ -5624,12 +5624,12 @@
       </c>
       <c r="W59" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>78</t>
         </is>
       </c>
       <c r="X59" t="inlineStr">
         <is>
-          <t>861=</t>
+          <t>864=</t>
         </is>
       </c>
       <c r="Y59" t="inlineStr"/>
@@ -6004,12 +6004,12 @@
       </c>
       <c r="W63" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>78</t>
         </is>
       </c>
       <c r="X63" t="inlineStr">
         <is>
-          <t>861=</t>
+          <t>864=</t>
         </is>
       </c>
       <c r="Y63" t="inlineStr"/>
@@ -6095,7 +6095,7 @@
       <c r="W64" t="inlineStr"/>
       <c r="X64" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>164</t>
         </is>
       </c>
       <c r="Y64" t="inlineStr"/>
@@ -6435,7 +6435,7 @@
       </c>
       <c r="X68" t="inlineStr">
         <is>
-          <t>551=</t>
+          <t>547=</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr"/>
@@ -6524,7 +6524,7 @@
       </c>
       <c r="W69" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="X69" t="inlineStr"/>
@@ -6620,7 +6620,7 @@
       </c>
       <c r="W70" t="inlineStr">
         <is>
-          <t>633</t>
+          <t>631</t>
         </is>
       </c>
       <c r="X70" t="inlineStr"/>
@@ -6811,7 +6811,7 @@
       </c>
       <c r="X72" t="inlineStr">
         <is>
-          <t>551=</t>
+          <t>547=</t>
         </is>
       </c>
       <c r="Y72" t="inlineStr"/>
@@ -6976,7 +6976,7 @@
       </c>
       <c r="W74" t="inlineStr">
         <is>
-          <t>633</t>
+          <t>631</t>
         </is>
       </c>
       <c r="X74" t="inlineStr"/>
@@ -7148,12 +7148,12 @@
       </c>
       <c r="W76" t="inlineStr">
         <is>
-          <t>1017</t>
+          <t>1019</t>
         </is>
       </c>
       <c r="X76" t="inlineStr">
         <is>
-          <t>1582=</t>
+          <t>1576=</t>
         </is>
       </c>
       <c r="Y76" t="inlineStr"/>
@@ -7335,7 +7335,7 @@
       </c>
       <c r="X78" t="inlineStr">
         <is>
-          <t>859</t>
+          <t>862</t>
         </is>
       </c>
       <c r="Y78" t="inlineStr"/>
@@ -7424,12 +7424,12 @@
       </c>
       <c r="W79" t="inlineStr">
         <is>
-          <t>1163</t>
+          <t>1194</t>
         </is>
       </c>
       <c r="X79" t="inlineStr">
         <is>
-          <t>1371=</t>
+          <t>1364=</t>
         </is>
       </c>
       <c r="Y79" t="inlineStr"/>
@@ -7518,12 +7518,12 @@
       </c>
       <c r="W80" t="inlineStr">
         <is>
-          <t>1017</t>
+          <t>1019</t>
         </is>
       </c>
       <c r="X80" t="inlineStr">
         <is>
-          <t>1582=</t>
+          <t>1576=</t>
         </is>
       </c>
       <c r="Y80" t="inlineStr">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="AA80" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>286</t>
         </is>
       </c>
       <c r="AB80" t="n">
@@ -7624,12 +7624,12 @@
       </c>
       <c r="W81" t="inlineStr">
         <is>
-          <t>1163</t>
+          <t>1194</t>
         </is>
       </c>
       <c r="X81" t="inlineStr">
         <is>
-          <t>1371=</t>
+          <t>1364=</t>
         </is>
       </c>
       <c r="Y81" t="inlineStr">
@@ -7718,12 +7718,12 @@
       </c>
       <c r="W82" t="inlineStr">
         <is>
-          <t>1163</t>
+          <t>1194</t>
         </is>
       </c>
       <c r="X82" t="inlineStr">
         <is>
-          <t>1371=</t>
+          <t>1364=</t>
         </is>
       </c>
       <c r="Y82" t="inlineStr"/>
@@ -7813,7 +7813,7 @@
       </c>
       <c r="X83" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>286</t>
         </is>
       </c>
       <c r="Y83" t="inlineStr"/>
@@ -7901,7 +7901,7 @@
       </c>
       <c r="X84" t="inlineStr">
         <is>
-          <t>859</t>
+          <t>862</t>
         </is>
       </c>
       <c r="Y84" t="inlineStr"/>
@@ -7984,7 +7984,7 @@
       </c>
       <c r="W85" t="inlineStr">
         <is>
-          <t>282</t>
+          <t>278</t>
         </is>
       </c>
       <c r="X85" t="inlineStr">
@@ -8961,7 +8961,7 @@
       </c>
       <c r="X96" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="Y96" t="inlineStr"/>
@@ -9300,7 +9300,7 @@
       </c>
       <c r="AA100" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="AB100" t="n">
@@ -9471,7 +9471,7 @@
       </c>
       <c r="X102" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="Y102" t="inlineStr"/>
@@ -9796,7 +9796,7 @@
       </c>
       <c r="W106" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="X106" t="inlineStr"/>
@@ -9889,7 +9889,7 @@
       <c r="W107" t="inlineStr"/>
       <c r="X107" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>164</t>
         </is>
       </c>
       <c r="Y107" t="inlineStr"/>
@@ -10159,7 +10159,7 @@
       </c>
       <c r="Z110" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="AA110" t="inlineStr"/>
@@ -10253,7 +10253,7 @@
       <c r="W111" t="inlineStr"/>
       <c r="X111" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>164</t>
         </is>
       </c>
       <c r="Y111" t="inlineStr">
@@ -10264,7 +10264,7 @@
       <c r="Z111" t="inlineStr"/>
       <c r="AA111" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>57</t>
         </is>
       </c>
       <c r="AB111" t="n">
@@ -10350,7 +10350,7 @@
       </c>
       <c r="W112" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="X112" t="inlineStr"/>
@@ -10613,7 +10613,7 @@
       <c r="W115" t="inlineStr"/>
       <c r="X115" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>164</t>
         </is>
       </c>
       <c r="Y115" t="inlineStr"/>
@@ -10694,7 +10694,7 @@
       </c>
       <c r="W116" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>136</t>
         </is>
       </c>
       <c r="X116" t="inlineStr"/>
@@ -10932,12 +10932,12 @@
       </c>
       <c r="W119" t="inlineStr">
         <is>
-          <t>1163</t>
+          <t>1194</t>
         </is>
       </c>
       <c r="X119" t="inlineStr">
         <is>
-          <t>1371=</t>
+          <t>1364=</t>
         </is>
       </c>
       <c r="Y119" t="inlineStr"/>
@@ -11028,7 +11028,7 @@
       </c>
       <c r="W120" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>136</t>
         </is>
       </c>
       <c r="X120" t="inlineStr"/>
@@ -11280,7 +11280,7 @@
       </c>
       <c r="W123" t="inlineStr">
         <is>
-          <t>282</t>
+          <t>278</t>
         </is>
       </c>
       <c r="X123" t="inlineStr">
@@ -11448,12 +11448,12 @@
       </c>
       <c r="W125" t="inlineStr">
         <is>
-          <t>1163</t>
+          <t>1194</t>
         </is>
       </c>
       <c r="X125" t="inlineStr">
         <is>
-          <t>1371=</t>
+          <t>1364=</t>
         </is>
       </c>
       <c r="Y125" t="inlineStr"/>
@@ -11710,7 +11710,7 @@
       </c>
       <c r="W128" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="X128" t="inlineStr"/>
@@ -11801,7 +11801,7 @@
       </c>
       <c r="X129" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="Y129" t="inlineStr"/>
@@ -11901,7 +11901,7 @@
       </c>
       <c r="Z130" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="AA130" t="inlineStr"/>
@@ -12008,7 +12008,7 @@
       </c>
       <c r="AA131" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="AB131" t="n">
@@ -12181,7 +12181,7 @@
       </c>
       <c r="X133" t="inlineStr">
         <is>
-          <t>832</t>
+          <t>840</t>
         </is>
       </c>
       <c r="Y133" t="inlineStr"/>
@@ -12508,7 +12508,7 @@
       </c>
       <c r="W137" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="X137" t="inlineStr"/>
@@ -12761,7 +12761,7 @@
       </c>
       <c r="Z140" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>136</t>
         </is>
       </c>
       <c r="AA140" t="inlineStr"/>
@@ -12851,7 +12851,7 @@
       </c>
       <c r="Z141" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>176</t>
         </is>
       </c>
       <c r="AA141" t="inlineStr"/>
@@ -12930,7 +12930,7 @@
       </c>
       <c r="W142" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>136</t>
         </is>
       </c>
       <c r="X142" t="inlineStr"/>

</xml_diff>